<commit_message>
Updated weapons to match game version 6.0.0
</commit_message>
<xml_diff>
--- a/splatoon_weapons.xlsx
+++ b/splatoon_weapons.xlsx
@@ -783,7 +783,7 @@
         <v>65</v>
       </c>
       <c r="W4" t="n">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5">
@@ -1138,7 +1138,7 @@
         <v>40</v>
       </c>
       <c r="W9" t="n">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10">
@@ -1351,7 +1351,7 @@
         <v>30</v>
       </c>
       <c r="W12" t="n">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13">
@@ -3262,13 +3262,13 @@
         </is>
       </c>
       <c r="P39" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="V39" t="n">
         <v>70</v>
       </c>
       <c r="W39" t="n">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40">
@@ -3546,7 +3546,7 @@
         </is>
       </c>
       <c r="P43" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="V43" t="n">
         <v>70</v>
@@ -3830,7 +3830,7 @@
         </is>
       </c>
       <c r="P47" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V47" t="n">
         <v>60</v>
@@ -3907,7 +3907,7 @@
         <v>60</v>
       </c>
       <c r="W48" t="n">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49">
@@ -4049,7 +4049,7 @@
         <v>65</v>
       </c>
       <c r="W50" t="n">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51">
@@ -4830,7 +4830,7 @@
         <v>90</v>
       </c>
       <c r="W61" t="n">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="62">
@@ -4895,13 +4895,13 @@
         </is>
       </c>
       <c r="P62" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="S62" t="n">
         <v>60</v>
       </c>
       <c r="W62" t="n">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="63">
@@ -5469,7 +5469,7 @@
         <v>30</v>
       </c>
       <c r="W70" t="n">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71">
@@ -5540,7 +5540,7 @@
         <v>65</v>
       </c>
       <c r="W71" t="n">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72">
@@ -5676,13 +5676,13 @@
         </is>
       </c>
       <c r="P73" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="S73" t="n">
         <v>75</v>
       </c>
       <c r="W73" t="n">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74">
@@ -5747,7 +5747,7 @@
         </is>
       </c>
       <c r="P74" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="S74" t="n">
         <v>75</v>
@@ -5818,7 +5818,7 @@
         </is>
       </c>
       <c r="P75" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="S75" t="n">
         <v>75</v>
@@ -5960,7 +5960,7 @@
         </is>
       </c>
       <c r="P77" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="S77" t="n">
         <v>75</v>
@@ -6173,7 +6173,7 @@
         </is>
       </c>
       <c r="P80" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="S80" t="n">
         <v>60</v>
@@ -6392,7 +6392,7 @@
         <v>30</v>
       </c>
       <c r="W83" t="n">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="84">
@@ -7173,7 +7173,7 @@
         <v>70</v>
       </c>
       <c r="W94" t="n">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95">
@@ -7315,7 +7315,7 @@
         <v>60</v>
       </c>
       <c r="W96" t="n">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="97">
@@ -7528,7 +7528,7 @@
         <v>60</v>
       </c>
       <c r="W99" t="n">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="100">
@@ -7954,7 +7954,7 @@
         <v>90</v>
       </c>
       <c r="W105" t="n">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="106">
@@ -8380,7 +8380,7 @@
         <v>40</v>
       </c>
       <c r="W111" t="n">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>